<commit_message>
AUTO FROM HOME 29.12.2022 23:55:28,04
</commit_message>
<xml_diff>
--- a/BOTVA-122022/сводка.xlsx
+++ b/BOTVA-122022/сводка.xlsx
@@ -585,13 +585,13 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,14 +913,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="I1" s="6" t="s">
         <v>162</v>
       </c>
@@ -978,7 +978,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="7"/>
+      <c r="I3" s="5"/>
       <c r="J3">
         <v>4</v>
       </c>
@@ -1011,16 +1011,16 @@
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="J4">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L4">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1045,7 +1045,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
       <c r="I5" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="J5">
         <v>40</v>
@@ -1079,16 +1079,16 @@
       <c r="G6" s="1"/>
       <c r="H6" s="2"/>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>120</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L6">
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1113,16 +1113,16 @@
       <c r="G7" s="1"/>
       <c r="H7" s="2"/>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>138</v>
       </c>
       <c r="J7">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="K7">
         <v>4</v>
       </c>
       <c r="L7">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1147,16 +1147,16 @@
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
       <c r="I8" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="J8">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1181,16 +1181,16 @@
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J9">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="K9">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1215,16 +1215,16 @@
       <c r="G10" s="1"/>
       <c r="H10" s="2"/>
       <c r="I10" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="J10">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L10">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1249,16 +1249,16 @@
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
       <c r="I11" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="J11">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="K11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L11">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1283,16 +1283,16 @@
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
       <c r="I12" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="J12">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L12">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1317,16 +1317,16 @@
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="J13">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="K13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1351,16 +1351,16 @@
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
       <c r="I14" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="J14">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1385,16 +1385,16 @@
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
       <c r="I15" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1419,16 +1419,16 @@
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
       <c r="I16" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="J16">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L16">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1453,16 +1453,16 @@
       <c r="G17" s="1"/>
       <c r="H17" s="2"/>
       <c r="I17" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="J17">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L17">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1487,16 +1487,16 @@
       <c r="G18" s="1"/>
       <c r="H18" s="2"/>
       <c r="I18" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="J18">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L18">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1521,16 +1521,16 @@
       <c r="G19" s="1"/>
       <c r="H19" s="2"/>
       <c r="I19" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="J19">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L19">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1555,7 +1555,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="2"/>
       <c r="I20" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="J20">
         <v>29</v>
@@ -1589,16 +1589,16 @@
       <c r="G21" s="1"/>
       <c r="H21" s="2"/>
       <c r="I21" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J21">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L21">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1623,16 +1623,16 @@
       <c r="G22" s="1"/>
       <c r="H22" s="2"/>
       <c r="I22" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="J22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1657,16 +1657,16 @@
       <c r="G23" s="1"/>
       <c r="H23" s="2"/>
       <c r="I23" t="s">
-        <v>129</v>
+        <v>16</v>
       </c>
       <c r="J23">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1691,16 +1691,16 @@
       <c r="G24" s="1"/>
       <c r="H24" s="2"/>
       <c r="I24" t="s">
-        <v>150</v>
+        <v>96</v>
       </c>
       <c r="J24">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="K24">
         <v>6</v>
       </c>
       <c r="L24">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1725,16 +1725,16 @@
       <c r="G25" s="1"/>
       <c r="H25" s="2"/>
       <c r="I25" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="J25">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1759,16 +1759,16 @@
       <c r="G26" s="1"/>
       <c r="H26" s="2"/>
       <c r="I26" t="s">
-        <v>144</v>
+        <v>10</v>
       </c>
       <c r="J26">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K26">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L26">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1793,16 +1793,16 @@
       <c r="G27" s="1"/>
       <c r="H27" s="2"/>
       <c r="I27" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="J27">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
       <c r="L27">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1827,16 +1827,16 @@
       <c r="G28" s="1"/>
       <c r="H28" s="2"/>
       <c r="I28" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="J28">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1861,16 +1861,16 @@
       <c r="G29" s="1"/>
       <c r="H29" s="2"/>
       <c r="I29" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="J29">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L29">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1895,16 +1895,16 @@
       <c r="G30" s="1"/>
       <c r="H30" s="2"/>
       <c r="I30" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="J30">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="K30">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L30">
-        <v>46</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1929,16 +1929,16 @@
       <c r="G31" s="1"/>
       <c r="H31" s="2"/>
       <c r="I31" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J31">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="K31">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L31">
-        <v>50</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1963,16 +1963,16 @@
       <c r="G32" s="1"/>
       <c r="H32" s="2"/>
       <c r="I32" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L32">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -1997,16 +1997,16 @@
       <c r="G33" s="1"/>
       <c r="H33" s="2"/>
       <c r="I33" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="J33">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="K33">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L33">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2031,16 +2031,16 @@
       <c r="G34" s="1"/>
       <c r="H34" s="2"/>
       <c r="I34" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="J34">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="K34">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L34">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2065,16 +2065,16 @@
       <c r="G35" s="1"/>
       <c r="H35" s="2"/>
       <c r="I35" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="J35">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K35">
         <v>0</v>
       </c>
       <c r="L35">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2099,16 +2099,16 @@
       <c r="G36" s="1"/>
       <c r="H36" s="2"/>
       <c r="I36" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="J36">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K36">
         <v>0</v>
       </c>
       <c r="L36">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2133,16 +2133,16 @@
       <c r="G37" s="1"/>
       <c r="H37" s="2"/>
       <c r="I37" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="J37">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K37">
         <v>0</v>
       </c>
       <c r="L37">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2167,16 +2167,16 @@
       <c r="G38" s="1"/>
       <c r="H38" s="2"/>
       <c r="I38" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="J38">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="K38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L38">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2201,16 +2201,16 @@
       <c r="G39" s="1"/>
       <c r="H39" s="2"/>
       <c r="I39" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="J39">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K39">
         <v>0</v>
       </c>
       <c r="L39">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2235,16 +2235,16 @@
       <c r="G40" s="1"/>
       <c r="H40" s="2"/>
       <c r="I40" t="s">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="J40">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="K40">
         <v>0</v>
       </c>
       <c r="L40">
-        <v>32</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2269,16 +2269,16 @@
       <c r="G41" s="1"/>
       <c r="H41" s="2"/>
       <c r="I41" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="J41">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
-        <v>32</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2303,16 +2303,16 @@
       <c r="G42" s="1"/>
       <c r="H42" s="2"/>
       <c r="I42" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="J42">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="K42">
         <v>0</v>
       </c>
       <c r="L42">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2337,16 +2337,16 @@
       <c r="G43" s="1"/>
       <c r="H43" s="2"/>
       <c r="I43" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="J43">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="K43">
         <v>0</v>
       </c>
       <c r="L43">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2371,16 +2371,16 @@
       <c r="G44" s="1"/>
       <c r="H44" s="2"/>
       <c r="I44" t="s">
-        <v>147</v>
+        <v>50</v>
       </c>
       <c r="J44">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="K44">
         <v>0</v>
       </c>
       <c r="L44">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2405,16 +2405,16 @@
       <c r="G45" s="1"/>
       <c r="H45" s="2"/>
       <c r="I45" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="J45">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2439,16 +2439,16 @@
       <c r="G46" s="1"/>
       <c r="H46" s="2"/>
       <c r="I46" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="J46">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="K46">
         <v>0</v>
       </c>
       <c r="L46">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2804,8 +2804,8 @@
       <c r="H62" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F62">
-    <sortCondition ref="A2:A62"/>
+  <sortState ref="I4:L46">
+    <sortCondition descending="1" ref="L4:L46"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="I1:L1"/>

</xml_diff>